<commit_message>
#ERM-15 Add all the columns deom the import while exporting success data
</commit_message>
<xml_diff>
--- a/UserManagement/wwwroot/UserRegistrationTemplate.xlsx
+++ b/UserManagement/wwwroot/UserRegistrationTemplate.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miAL1z3bwJq/lBXPujJBU0yWJ5Ijg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mh4NX+ISiwfCu4qLlV4gWPXKkmvuQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
   <si>
     <r>
       <rPr>
@@ -144,13 +144,13 @@
     <t>Assign PHC Or Hub</t>
   </si>
   <si>
-    <t>HSC Rajesh</t>
-  </si>
-  <si>
-    <t>SubCentre</t>
-  </si>
-  <si>
-    <t>rajeshcdac@gmail.com</t>
+    <t>HUB Kerry12</t>
+  </si>
+  <si>
+    <t>HUB</t>
+  </si>
+  <si>
+    <t>Kerry12@gmail.com</t>
   </si>
   <si>
     <t>RAJASTHAN</t>
@@ -162,10 +162,10 @@
     <t>ABU ROAD</t>
   </si>
   <si>
-    <t>rajesh</t>
-  </si>
-  <si>
-    <t>Kumar</t>
+    <t>Mohit11</t>
+  </si>
+  <si>
+    <t>Joshi1</t>
   </si>
   <si>
     <t>Male</t>
@@ -174,13 +174,22 @@
     <t>GNM</t>
   </si>
   <si>
-    <t>rajesh121@cdac.com</t>
+    <t>Mohit11Joshi11@cdac.com</t>
   </si>
   <si>
     <t>CHO</t>
   </si>
   <si>
-    <t>10-10-1981</t>
+    <t>10-06-1982</t>
+  </si>
+  <si>
+    <t>WEST BENGAL</t>
+  </si>
+  <si>
+    <t>24 PARAGANAS NORTH</t>
+  </si>
+  <si>
+    <t>AMDANGA</t>
   </si>
   <si>
     <t>Dr</t>
@@ -192,34 +201,31 @@
     <t>GMC Clinic</t>
   </si>
   <si>
-    <t>HSC ABOHAR1</t>
-  </si>
-  <si>
-    <t>faiabhor1@gmail.com</t>
-  </si>
-  <si>
-    <t>PUNJAB</t>
-  </si>
-  <si>
-    <t>FAZILKA</t>
+    <t>UPHC Debbe12</t>
+  </si>
+  <si>
+    <t>UPHC</t>
+  </si>
+  <si>
+    <t>Debbe12@gmail.com</t>
+  </si>
+  <si>
+    <t>Guneet11</t>
+  </si>
+  <si>
+    <t>Wagh</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Guneet11Wagh1@gmail.com</t>
+  </si>
+  <si>
+    <t>KOLKATA</t>
   </si>
   <si>
     <t>ABOHAR</t>
-  </si>
-  <si>
-    <t>ABHOR</t>
-  </si>
-  <si>
-    <t>Faizal</t>
-  </si>
-  <si>
-    <t>aaaa</t>
-  </si>
-  <si>
-    <t>faizal111@gmail.com</t>
-  </si>
-  <si>
-    <t>10-06-1982</t>
   </si>
   <si>
     <t>HWC Majra</t>
@@ -284,17 +290,15 @@
       <b/>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Docs-calibri"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -391,50 +395,50 @@
     <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -776,7 +780,7 @@
       <c r="Q2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="10" t="s">
         <v>19</v>
       </c>
       <c r="S2" s="7" t="s">
@@ -797,31 +801,31 @@
       <c r="X2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Y2" s="11" t="s">
         <v>26</v>
       </c>
       <c r="Z2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AA2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="11" t="s">
+      <c r="AB2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AC2" s="11" t="s">
+      <c r="AC2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="AD2" s="11" t="s">
+      <c r="AD2" s="12" t="s">
         <v>31</v>
       </c>
       <c r="AE2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AF2" s="8" t="s">
+      <c r="AF2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AG2" s="8" t="s">
+      <c r="AG2" s="11" t="s">
         <v>34</v>
       </c>
     </row>
@@ -829,270 +833,202 @@
       <c r="A3" s="5">
         <v>1.0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="5">
         <v>2.9382939E7</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="14">
         <v>3.409203E7</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="15" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="14">
         <v>87299.0</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="13" t="s">
         <v>41</v>
       </c>
       <c r="M3" s="17" t="s">
         <v>42</v>
       </c>
       <c r="N3" s="18">
-        <v>9.228822877E9</v>
-      </c>
-      <c r="O3" s="12" t="s">
+        <v>9.434954873E9</v>
+      </c>
+      <c r="O3" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="Q3" s="18">
+      <c r="Q3" s="20">
         <v>19.0</v>
       </c>
       <c r="R3" s="5">
         <v>2.3929999E7</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="S3" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="V3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="W3" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="X3" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y3" s="15" t="s">
+      <c r="V3" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="X3" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y3" s="16" t="s">
         <v>40</v>
       </c>
       <c r="Z3" s="5">
         <v>989999.0</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC3" s="19">
-        <v>0.395833333333333</v>
-      </c>
-      <c r="AD3" s="19">
+        <v>52</v>
+      </c>
+      <c r="AC3" s="23">
+        <v>0.3958333333333333</v>
+      </c>
+      <c r="AD3" s="24">
         <v>0.916666666666667</v>
       </c>
       <c r="AE3" s="5">
         <v>3.0</v>
       </c>
       <c r="AF3" s="5"/>
-      <c r="AG3" s="15" t="s">
-        <v>50</v>
+      <c r="AG3" s="16" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5">
         <v>2.0</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>51</v>
+      <c r="B4" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="C4" s="5">
-        <v>2.399023E7</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="13">
-        <v>1.2345678E7</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="15" t="s">
+        <v>2.9382939E7</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="E4" s="14">
+        <v>3.409203E7</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="13">
-        <v>122233.0</v>
-      </c>
-      <c r="L4" s="12" t="s">
+      <c r="G4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="14">
+        <v>87299.0</v>
+      </c>
+      <c r="L4" s="13" t="s">
         <v>57</v>
       </c>
       <c r="M4" s="17" t="s">
         <v>58</v>
       </c>
       <c r="N4" s="18">
-        <v>8.438057323E9</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="P4" s="12" t="s">
+        <v>8.633462355E9</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="Q4" s="18">
+      <c r="Q4" s="20">
         <v>19.0</v>
       </c>
       <c r="R4" s="5">
         <v>2.3989839E7</v>
       </c>
-      <c r="S4" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="T4" s="12" t="s">
+      <c r="S4" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="T4" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="U4" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="V4" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="W4" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="X4" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y4" s="15" t="s">
-        <v>55</v>
+      <c r="U4" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="V4" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="W4" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="X4" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y4" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="Z4" s="5">
         <v>120900.0</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="AB4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC4" s="19">
+        <v>52</v>
+      </c>
+      <c r="AC4" s="24">
         <v>0.395833333333333</v>
       </c>
-      <c r="AD4" s="19">
+      <c r="AD4" s="24">
         <v>0.916666666666667</v>
       </c>
       <c r="AE4" s="5">
         <v>3.0</v>
       </c>
       <c r="AF4" s="5"/>
-      <c r="AG4" s="15" t="s">
-        <v>61</v>
+      <c r="AG4" s="16" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="22"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="19"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5"/>
-      <c r="AG5" s="15"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="5"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="5"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="19"/>
-      <c r="AE6" s="5"/>
-      <c r="AF6" s="5"/>
-      <c r="AG6" s="15"/>
-    </row>
+    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
@@ -2071,8 +2007,6 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:K1"/>

</xml_diff>

<commit_message>
#ERM-15 Add all the columns from the import while exporting error data
</commit_message>
<xml_diff>
--- a/UserManagement/wwwroot/UserRegistrationTemplate.xlsx
+++ b/UserManagement/wwwroot/UserRegistrationTemplate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
   <si>
     <r>
       <rPr>
@@ -144,13 +144,13 @@
     <t>Assign PHC Or Hub</t>
   </si>
   <si>
-    <t>HUB Kerry12</t>
+    <t>HUB Kerry</t>
   </si>
   <si>
     <t>HUB</t>
   </si>
   <si>
-    <t>Kerry12@gmail.com</t>
+    <t>Kerry@gmail.com</t>
   </si>
   <si>
     <t>RAJASTHAN</t>
@@ -162,10 +162,10 @@
     <t>ABU ROAD</t>
   </si>
   <si>
-    <t>Mohit11</t>
-  </si>
-  <si>
-    <t>Joshi1</t>
+    <t>Mohit</t>
+  </si>
+  <si>
+    <t>Joshi</t>
   </si>
   <si>
     <t>Male</t>
@@ -174,7 +174,7 @@
     <t>GNM</t>
   </si>
   <si>
-    <t>Mohit11Joshi11@cdac.com</t>
+    <t>Mohit@cdac.com</t>
   </si>
   <si>
     <t>CHO</t>
@@ -198,19 +198,25 @@
     <t>Monday,Sunday</t>
   </si>
   <si>
+    <t>9:30 AM</t>
+  </si>
+  <si>
+    <t>10:00 PM</t>
+  </si>
+  <si>
     <t>GMC Clinic</t>
   </si>
   <si>
-    <t>UPHC Debbe12</t>
+    <t>UPHC Debbe</t>
   </si>
   <si>
     <t>UPHC</t>
   </si>
   <si>
-    <t>Debbe12@gmail.com</t>
-  </si>
-  <si>
-    <t>Guneet11</t>
+    <t>Debbe@gmail.com</t>
+  </si>
+  <si>
+    <t>Guneet</t>
   </si>
   <si>
     <t>Wagh</t>
@@ -219,7 +225,7 @@
     <t>Female</t>
   </si>
   <si>
-    <t>Guneet11Wagh1@gmail.com</t>
+    <t>Guneet@gmail.com</t>
   </si>
   <si>
     <t>KOLKATA</t>
@@ -235,9 +241,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-C09]H:MM\ AM/PM"/>
-  </numFmts>
   <fonts count="12">
     <font>
       <sz val="11.0"/>
@@ -431,14 +434,14 @@
     <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -870,7 +873,7 @@
         <v>42</v>
       </c>
       <c r="N3" s="18">
-        <v>9.434954873E9</v>
+        <v>9.434454873E9</v>
       </c>
       <c r="O3" s="13" t="s">
         <v>43</v>
@@ -914,18 +917,18 @@
       <c r="AB3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AC3" s="23">
-        <v>0.3958333333333333</v>
-      </c>
-      <c r="AD3" s="24">
-        <v>0.916666666666667</v>
+      <c r="AC3" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD3" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="AE3" s="5">
         <v>3.0</v>
       </c>
       <c r="AF3" s="5"/>
       <c r="AG3" s="16" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
@@ -933,19 +936,19 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C4" s="5">
         <v>2.9382939E7</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E4" s="14">
         <v>3.409203E7</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>38</v>
@@ -963,16 +966,16 @@
         <v>87299.0</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N4" s="18">
-        <v>8.633462355E9</v>
+        <v>8.632362355E9</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="P4" s="13" t="s">
         <v>44</v>
@@ -984,7 +987,7 @@
         <v>2.3989839E7</v>
       </c>
       <c r="S4" s="13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="T4" s="19" t="s">
         <v>46</v>
@@ -995,14 +998,14 @@
       <c r="V4" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="W4" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="X4" s="25" t="s">
-        <v>61</v>
+      <c r="W4" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="X4" s="24" t="s">
+        <v>63</v>
       </c>
       <c r="Y4" s="16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Z4" s="5">
         <v>120900.0</v>
@@ -1013,18 +1016,18 @@
       <c r="AB4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AC4" s="24">
-        <v>0.395833333333333</v>
-      </c>
-      <c r="AD4" s="24">
-        <v>0.916666666666667</v>
+      <c r="AC4" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD4" s="25" t="s">
+        <v>54</v>
       </c>
       <c r="AE4" s="5">
         <v>3.0</v>
       </c>
       <c r="AF4" s="5"/>
       <c r="AG4" s="16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1"/>

</xml_diff>